<commit_message>
Ajout du context pour les extensions 275a48ab645cc3de35f2b7c35c981c21ab98daa8
</commit_message>
<xml_diff>
--- a/302-contenu-fhir---ajout-des-données-usager/ig/StructureDefinition-tddui-birth-order.xlsx
+++ b/302-contenu-fhir---ajout-des-données-usager/ig/StructureDefinition-tddui-birth-order.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-07-18T12:58:08+00:00</t>
+    <t>2025-07-18T13:16:41+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -129,7 +129,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:Element</t>
+    <t>element:Patient</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>